<commit_message>
Notes on other top performers
</commit_message>
<xml_diff>
--- a/paper/biosnap_papers.xlsx
+++ b/paper/biosnap_papers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fu19841/Documents/thesis_analysis/Chapter2/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8B420C-D57F-164B-A18F-06EDF42948FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D37291-60D2-1943-8B31-D0DF013506F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="500" windowWidth="26960" windowHeight="16940" xr2:uid="{E12F268A-15B5-0947-8C72-D82EE4B297FC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="58">
   <si>
     <t>Mechanism</t>
   </si>
@@ -192,6 +192,24 @@
   </si>
   <si>
     <t>scores are best of the model from the three 'tasks' on the same dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">800 epochs, uses enzyme and drug transporter data, </t>
+  </si>
+  <si>
+    <t>120 epochs, uses atomic structure data in 'graph of graphs' format</t>
+  </si>
+  <si>
+    <t>Suspicious results. Model is decagon, extended with relation attention module.</t>
+  </si>
+  <si>
+    <t>Enzyme and transporter data, also removed ~100 drugs from decagon data</t>
+  </si>
+  <si>
+    <t>SAME DATA/AUTHORS AS MS-ADR</t>
+  </si>
+  <si>
+    <t>Chemical substructure data</t>
   </si>
 </sst>
 </file>
@@ -546,7 +564,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -589,19 +607,22 @@
       <c r="D2">
         <v>0.998</v>
       </c>
+      <c r="F2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>29</v>
       </c>
       <c r="C3">
-        <v>0.97299999999999998</v>
-      </c>
-      <c r="D3">
-        <v>0.98299999999999998</v>
+        <v>0.99</v>
+      </c>
+      <c r="F3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -617,143 +638,152 @@
       <c r="D4">
         <v>0.98</v>
       </c>
+      <c r="F4" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C5">
-        <v>0.95499999999999996</v>
+        <v>0.97799999999999998</v>
       </c>
       <c r="D5">
-        <v>0.97199999999999998</v>
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="E5">
+        <v>0.98</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C6">
-        <v>0.97799999999999998</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="D6">
-        <v>0.97099999999999997</v>
-      </c>
-      <c r="E6">
-        <v>0.98</v>
+        <v>0.96799999999999997</v>
+      </c>
+      <c r="F6" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="C7">
-        <v>0.97499999999999998</v>
+        <v>0.97299999999999998</v>
       </c>
       <c r="D7">
-        <v>0.96799999999999997</v>
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="F7" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="C8">
-        <v>0.96250000000000002</v>
+        <v>0.96599999999999997</v>
       </c>
       <c r="D8">
-        <v>0.96530000000000005</v>
+        <v>0.95299999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
         <v>29</v>
       </c>
       <c r="C9">
-        <v>0.95699999999999996</v>
+        <v>0.96250000000000002</v>
       </c>
       <c r="D9">
-        <v>0.96499999999999997</v>
-      </c>
-      <c r="E9">
-        <v>0.96699999999999997</v>
-      </c>
-      <c r="F9" t="s">
-        <v>31</v>
+        <v>0.96530000000000005</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>0.96</v>
       </c>
       <c r="D10">
-        <v>0.96</v>
-      </c>
-      <c r="F10" t="s">
-        <v>40</v>
+        <v>0.71</v>
+      </c>
+      <c r="E10">
+        <v>0.9</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
         <v>29</v>
       </c>
       <c r="C11">
-        <v>0.94830000000000003</v>
+        <v>0.95699999999999996</v>
       </c>
       <c r="D11">
-        <v>0.95309999999999995</v>
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="E11">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="F11" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="C12">
-        <v>0.96599999999999997</v>
-      </c>
-      <c r="D12">
-        <v>0.95299999999999996</v>
+        <v>0.95699999999999996</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
         <v>29</v>
       </c>
       <c r="C13">
-        <v>0.93200000000000005</v>
+        <v>0.95499999999999996</v>
       </c>
       <c r="D13">
-        <v>0.93799999999999994</v>
+        <v>0.97199999999999998</v>
       </c>
       <c r="F13" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -772,246 +802,252 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
         <v>29</v>
       </c>
       <c r="C15">
-        <v>0.94699999999999995</v>
+        <v>0.94830000000000003</v>
       </c>
       <c r="D15">
-        <v>0.93</v>
-      </c>
-      <c r="E15">
-        <v>0.89500000000000002</v>
+        <v>0.95309999999999995</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="C16">
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="D16">
         <v>0.93</v>
       </c>
-      <c r="D16">
-        <v>0.92</v>
+      <c r="E16">
+        <v>0.89500000000000002</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="C17">
-        <v>0.88900000000000001</v>
-      </c>
-      <c r="D17">
-        <v>0.91500000000000004</v>
+        <v>0.93899999999999995</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
         <v>29</v>
       </c>
       <c r="C18">
-        <v>0.92800000000000005</v>
+        <v>0.93200000000000005</v>
       </c>
       <c r="D18">
-        <v>0.90200000000000002</v>
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="F18" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="C19">
-        <v>0.90100000000000002</v>
-      </c>
-      <c r="D19">
-        <v>0.89600000000000002</v>
-      </c>
-      <c r="E19">
-        <v>0.83199999999999996</v>
+        <v>0.93169999999999997</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
       </c>
       <c r="C20">
-        <v>0.91</v>
+        <v>0.93</v>
       </c>
       <c r="D20">
-        <v>0.88700000000000001</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C21">
-        <v>0.89900000000000002</v>
+        <v>0.92800000000000005</v>
       </c>
       <c r="D21">
-        <v>0.878</v>
-      </c>
-      <c r="E21">
-        <v>0.85699999999999998</v>
+        <v>0.90200000000000002</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C22">
-        <v>0.90300000000000002</v>
-      </c>
-      <c r="D22">
-        <v>0.875</v>
-      </c>
-      <c r="E22">
-        <v>0.86499999999999999</v>
-      </c>
-      <c r="F22" t="s">
-        <v>32</v>
+        <v>0.91490000000000005</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="C23">
-        <v>0.872</v>
+        <v>0.91</v>
       </c>
       <c r="D23">
-        <v>0.83199999999999996</v>
-      </c>
-      <c r="E23">
-        <v>0.80300000000000005</v>
-      </c>
-      <c r="F23" t="s">
-        <v>47</v>
+        <v>0.88700000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C24">
-        <v>0.82199999999999995</v>
+        <v>0.90300000000000002</v>
       </c>
       <c r="D24">
-        <v>0.77500000000000002</v>
+        <v>0.875</v>
+      </c>
+      <c r="E24">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="F24" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
       </c>
       <c r="C25">
-        <v>0.96</v>
+        <v>0.90100000000000002</v>
       </c>
       <c r="D25">
-        <v>0.71</v>
+        <v>0.89600000000000002</v>
       </c>
       <c r="E25">
-        <v>0.9</v>
+        <v>0.83199999999999996</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C26">
-        <v>0.99</v>
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="D26">
+        <v>0.878</v>
+      </c>
+      <c r="E26">
+        <v>0.85699999999999998</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="C27">
-        <v>0.95699999999999996</v>
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="D27">
+        <v>0.91500000000000004</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B28" t="s">
         <v>29</v>
       </c>
       <c r="C28">
-        <v>0.93899999999999995</v>
+        <v>0.872</v>
+      </c>
+      <c r="D28">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="E28">
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="F28" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
         <v>29</v>
       </c>
       <c r="C29">
-        <v>0.93169999999999997</v>
+        <v>0.86519999999999997</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
       </c>
       <c r="C30">
-        <v>0.91490000000000005</v>
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="D30">
+        <v>0.77500000000000002</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
         <v>29</v>
       </c>
-      <c r="C31">
-        <v>0.86519999999999997</v>
+      <c r="D31">
+        <v>0.96</v>
+      </c>
+      <c r="F31" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1051,7 +1087,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F35">
-    <sortCondition descending="1" ref="D1:D35"/>
+    <sortCondition descending="1" ref="C1:C35"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>